<commit_message>
Edits to comments on code and LM results table
</commit_message>
<xml_diff>
--- a/LM_results.xlsx
+++ b/LM_results.xlsx
@@ -8,19 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ae589d5c8305b1a1/Desktop/Tonga/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="11_BF0EB022D831E02E5212411A4190A93A77AD92FF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8DEE6AC0-FCEF-45BF-B380-AEB975D8B889}"/>
+  <xr:revisionPtr revIDLastSave="97" documentId="11_BF0EB022D831E02E5212411A4190A93A77AD92FF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{33DB0467-5C44-4C72-93EE-241A95DEE520}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="96">
   <si>
     <t/>
   </si>
@@ -269,13 +280,52 @@
   </si>
   <si>
     <t>Wetland</t>
+  </si>
+  <si>
+    <t>Site</t>
+  </si>
+  <si>
+    <t>Ngofe Marsh</t>
+  </si>
+  <si>
+    <t>Tephra</t>
+  </si>
+  <si>
+    <t>Avai'o'vuna Swamp</t>
+  </si>
+  <si>
+    <t>Lotofoa Swamp</t>
+  </si>
+  <si>
+    <t>Finemui Swamp</t>
+  </si>
+  <si>
+    <t>Coefficents</t>
+  </si>
+  <si>
+    <t>R2 values</t>
+  </si>
+  <si>
+    <t>R² = 0.3 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R² = 0.3 ** </t>
+  </si>
+  <si>
+    <t>R² = 0.7 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R² = 0.4 *  </t>
+  </si>
+  <si>
+    <t>R² = 0.4 ***</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -288,16 +338,61 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -359,11 +454,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -397,6 +521,69 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="5" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -694,15 +881,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U11"/>
+  <dimension ref="A1:U33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="21" width="10.6640625" customWidth="1"/>
+    <col min="1" max="1" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="21" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
@@ -930,68 +1118,68 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:21" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="13">
         <v>0.09</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="13">
         <v>0.12</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="13">
         <v>-0.19</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="13">
         <v>0.25</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="13">
         <v>-0.32</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="I5" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="J5" s="6">
+      <c r="J5" s="13">
         <v>-0.11</v>
       </c>
-      <c r="K5" s="6" t="s">
+      <c r="K5" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="L5" s="6">
+      <c r="L5" s="13">
         <v>0.54</v>
       </c>
-      <c r="M5" s="6">
+      <c r="M5" s="13">
         <v>-0.3</v>
       </c>
-      <c r="N5" s="6" t="s">
+      <c r="N5" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="O5" s="6">
+      <c r="O5" s="13">
         <v>0.04</v>
       </c>
-      <c r="P5" s="6" t="s">
+      <c r="P5" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="Q5" s="6">
+      <c r="Q5" s="13">
         <v>0.14000000000000001</v>
       </c>
-      <c r="R5" s="6" t="s">
+      <c r="R5" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="S5" s="6">
+      <c r="S5" s="13">
         <v>-0.06</v>
       </c>
-      <c r="T5" s="6">
+      <c r="T5" s="13">
         <v>0.28999999999999998</v>
       </c>
-      <c r="U5" s="6" t="s">
+      <c r="U5" s="13" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1060,68 +1248,68 @@
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:21" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="16">
         <v>-0.17</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="16">
         <v>-0.24</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="16">
         <v>-0.31</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="16">
         <v>1.1599999999999999</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="16">
         <v>0.87</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="16">
         <v>0.45</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="16">
         <v>-0.62</v>
       </c>
-      <c r="I7" s="6">
+      <c r="I7" s="16">
         <v>0.04</v>
       </c>
-      <c r="J7" s="6">
+      <c r="J7" s="16">
         <v>0.2</v>
       </c>
-      <c r="K7" s="6">
+      <c r="K7" s="16">
         <v>-0.01</v>
       </c>
-      <c r="L7" s="6">
+      <c r="L7" s="16">
         <v>-0.56999999999999995</v>
       </c>
-      <c r="M7" s="6">
+      <c r="M7" s="16">
         <v>-0.15</v>
       </c>
-      <c r="N7" s="6">
+      <c r="N7" s="16">
         <v>0.51</v>
       </c>
-      <c r="O7" s="6">
+      <c r="O7" s="16">
         <v>0.04</v>
       </c>
-      <c r="P7" s="6">
+      <c r="P7" s="16">
         <v>-1.94</v>
       </c>
-      <c r="Q7" s="6">
+      <c r="Q7" s="16">
         <v>0.57999999999999996</v>
       </c>
-      <c r="R7" s="6">
+      <c r="R7" s="16">
         <v>-0.06</v>
       </c>
-      <c r="S7" s="6">
+      <c r="S7" s="16">
         <v>-0.28999999999999998</v>
       </c>
-      <c r="T7" s="6">
+      <c r="T7" s="16">
         <v>-0.18</v>
       </c>
-      <c r="U7" s="6">
+      <c r="U7" s="16">
         <v>-0.28999999999999998</v>
       </c>
     </row>
@@ -1385,8 +1573,379 @@
         <v>6</v>
       </c>
     </row>
+    <row r="12" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2"/>
+      <c r="S12" s="2"/>
+      <c r="T12" s="2"/>
+      <c r="U12" s="2"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A13" s="31" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A14" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="B14" s="18"/>
+      <c r="C14" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="G14" s="18" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A15" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="21">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D15" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="E15" s="23">
+        <v>-0.06</v>
+      </c>
+      <c r="F15" s="23">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="G15" s="24" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A16" s="19"/>
+      <c r="B16" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="C16" s="25">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="D16" s="25">
+        <v>-0.06</v>
+      </c>
+      <c r="E16" s="25">
+        <v>-0.28999999999999998</v>
+      </c>
+      <c r="F16" s="25">
+        <v>-0.18</v>
+      </c>
+      <c r="G16" s="25">
+        <v>-0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="25">
+        <v>0.09</v>
+      </c>
+      <c r="D17" s="25">
+        <v>0.12</v>
+      </c>
+      <c r="E17" s="25">
+        <v>-0.19</v>
+      </c>
+      <c r="F17" s="25">
+        <v>0.25</v>
+      </c>
+      <c r="G17" s="25">
+        <v>-0.32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="19"/>
+      <c r="B18" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="C18" s="25">
+        <v>-0.17</v>
+      </c>
+      <c r="D18" s="25">
+        <v>-0.24</v>
+      </c>
+      <c r="E18" s="25">
+        <v>-0.31</v>
+      </c>
+      <c r="F18" s="25">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="G18" s="25">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="25">
+        <v>0.54</v>
+      </c>
+      <c r="D19" s="25">
+        <v>-0.3</v>
+      </c>
+      <c r="E19" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="F19" s="25">
+        <v>0.04</v>
+      </c>
+      <c r="G19" s="27" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="19"/>
+      <c r="B20" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="C20" s="25">
+        <v>-0.56999999999999995</v>
+      </c>
+      <c r="D20" s="25">
+        <v>-0.15</v>
+      </c>
+      <c r="E20" s="25">
+        <v>0.51</v>
+      </c>
+      <c r="F20" s="25">
+        <v>0.04</v>
+      </c>
+      <c r="G20" s="25">
+        <v>-1.94</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="E21" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="F21" s="25">
+        <v>-0.11</v>
+      </c>
+      <c r="G21" s="26" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="28"/>
+      <c r="B22" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="C22" s="30">
+        <v>0.45</v>
+      </c>
+      <c r="D22" s="30">
+        <v>-0.62</v>
+      </c>
+      <c r="E22" s="30">
+        <v>0.04</v>
+      </c>
+      <c r="F22" s="30">
+        <v>0.2</v>
+      </c>
+      <c r="G22" s="30">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="31" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="B25" s="18"/>
+      <c r="C25" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="D25" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="E25" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="F25" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="G25" s="18" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="B26" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26" s="21"/>
+      <c r="D26" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="E26" s="23"/>
+      <c r="F26" s="23"/>
+      <c r="G26" s="33" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="19"/>
+      <c r="B27" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="C27" s="25"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="25"/>
+      <c r="F27" s="25"/>
+      <c r="G27" s="25"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="B28" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="19"/>
+      <c r="B29" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="C29" s="25"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="25"/>
+      <c r="G29" s="25"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="B30" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C30" s="25"/>
+      <c r="D30" s="25"/>
+      <c r="E30" s="34" t="s">
+        <v>94</v>
+      </c>
+      <c r="F30" s="25"/>
+      <c r="G30" s="32" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="19"/>
+      <c r="B31" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="C31" s="25"/>
+      <c r="D31" s="25"/>
+      <c r="E31" s="25"/>
+      <c r="F31" s="25"/>
+      <c r="G31" s="25"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="B32" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="D32" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="E32" s="34" t="s">
+        <v>93</v>
+      </c>
+      <c r="F32" s="25"/>
+      <c r="G32" s="34" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" s="19"/>
+      <c r="B33" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="C33" s="25"/>
+      <c r="D33" s="25"/>
+      <c r="E33" s="25"/>
+      <c r="F33" s="25"/>
+      <c r="G33" s="25"/>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="13">
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A26:A27"/>
     <mergeCell ref="A11:U11"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="G1:K1"/>
@@ -1394,6 +1953,6 @@
     <mergeCell ref="Q1:U1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>